<commit_message>
v1.1 Changed the owner status
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_TC_NOTIFICATION_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_TC_NOTIFICATION_REVIEWS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ce4e295319cf0be1/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mego\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ACF53A5A-DF48-44F9-91EB-59CB83A00B01}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5610F983-6FC1-41AB-8257-2BEE6A1D492D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LH_TC_NOTIFICATION_REVIEWS" sheetId="2" r:id="rId1"/>
@@ -21,12 +21,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
   <si>
     <t>Author</t>
   </si>
@@ -164,6 +175,15 @@
   </si>
   <si>
     <t>Please ensure the test case ID follows the project's naming convention: it should begin with 'LH' and use hyphens (-) instead of underscores (_) to separate segments (LH-TC-SECTION-ID). Also ensure that the tab is named after the feature you are working with: (LH_TC_FEATURENAME).</t>
+  </si>
+  <si>
+    <t>v1.1</t>
+  </si>
+  <si>
+    <t>Changed the owner status</t>
+  </si>
+  <si>
+    <t>Closed</t>
   </si>
 </sst>
 </file>
@@ -273,6 +293,25 @@
   </cellStyles>
   <dxfs count="18">
     <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -284,20 +323,24 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
+        <right/>
         <top style="thin">
           <color indexed="64"/>
         </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -313,7 +356,7 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -326,6 +369,12 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -341,7 +390,7 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -354,6 +403,12 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -368,10 +423,11 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
         <right style="thin">
           <color indexed="64"/>
         </right>
@@ -395,7 +451,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -424,23 +480,19 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -524,7 +576,7 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -537,12 +589,6 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -557,11 +603,10 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
         <right style="thin">
           <color indexed="64"/>
         </right>
@@ -571,12 +616,6 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -621,25 +660,6 @@
           <color indexed="64"/>
         </horizontal>
       </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -655,31 +675,31 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:J12" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:J12" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Date" dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Review ID" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Reviewed Entity" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Reviewer" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Version" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Review Comments" dataDxfId="0"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Actions" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Owner" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Owner Status" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Reviewer verification" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Date" dataDxfId="15"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Review ID" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Reviewed Entity" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Reviewer" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Version" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Review Comments" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Actions" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Owner" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Owner Status" dataDxfId="7"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Reviewer verification" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:D9" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:D9" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Version Number" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Author" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Updated Section" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Date" dataDxfId="12">
-      <calculatedColumnFormula>DATE(2025,4,16)</calculatedColumnFormula>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Version Number" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Author" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Updated Section" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Date" dataDxfId="0">
+      <calculatedColumnFormula>DATE(2025,4,21)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -729,7 +749,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -781,7 +801,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -985,26 +1005,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="45.5703125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="36.7109375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="26.7109375" style="5" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="115.7109375" style="10" customWidth="1"/>
-    <col min="7" max="7" width="103.42578125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="28.28515625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="19.5703125" style="5" customWidth="1"/>
-    <col min="10" max="10" width="37.42578125" style="5" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="16.5546875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="45.5546875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="36.6640625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="26.6640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="21.109375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="115.6640625" style="10" customWidth="1"/>
+    <col min="7" max="7" width="103.44140625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="28.33203125" style="5" customWidth="1"/>
+    <col min="9" max="9" width="19.5546875" style="5" customWidth="1"/>
+    <col min="10" max="10" width="37.44140625" style="5" customWidth="1"/>
+    <col min="11" max="16384" width="9.109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -1036,7 +1056,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="84" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="84" x14ac:dyDescent="0.4">
       <c r="A2" s="11">
         <v>45768</v>
       </c>
@@ -1062,13 +1082,13 @@
         <v>18</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="J2" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="84" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="84" x14ac:dyDescent="0.4">
       <c r="A3" s="11">
         <v>45768</v>
       </c>
@@ -1094,13 +1114,13 @@
         <v>18</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="J3" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="105" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="105" x14ac:dyDescent="0.4">
       <c r="A4" s="11">
         <v>45768</v>
       </c>
@@ -1126,13 +1146,13 @@
         <v>18</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="J4" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A5" s="8"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -1144,7 +1164,7 @@
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A6" s="8"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -1156,7 +1176,7 @@
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A7" s="8"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -1168,7 +1188,7 @@
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A8" s="8"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -1180,7 +1200,7 @@
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A9" s="8"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -1192,7 +1212,7 @@
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A10" s="8"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -1204,7 +1224,7 @@
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A11" s="8"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -1216,7 +1236,7 @@
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A12" s="8"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -1228,10 +1248,10 @@
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A13" s="9"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A14" s="9"/>
     </row>
   </sheetData>
@@ -1260,18 +1280,18 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B5"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" customWidth="1"/>
-    <col min="3" max="3" width="36.5703125" customWidth="1"/>
+    <col min="1" max="1" width="25.109375" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" customWidth="1"/>
+    <col min="3" max="3" width="36.5546875" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -1285,7 +1305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1296,53 +1316,63 @@
         <v>3</v>
       </c>
       <c r="D2" s="4">
-        <f t="shared" ref="D2" si="0">DATE(2025,4,16)</f>
-        <v>45763</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="4"/>
-    </row>
-    <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <f t="shared" ref="D2:D9" si="0">DATE(2025,4,21)</f>
+        <v>45768</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="4">
+        <f t="shared" si="0"/>
+        <v>45768</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="4"/>
     </row>
-    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="4"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
v1.2 verified the notification test cases
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_TC_NOTIFICATION_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_TC_NOTIFICATION_REVIEWS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mego\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gehad\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5610F983-6FC1-41AB-8257-2BEE6A1D492D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4AF8873-362A-4939-A271-0A8D0DB8BF85}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LH_TC_NOTIFICATION_REVIEWS" sheetId="2" r:id="rId1"/>
@@ -21,23 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
   <si>
     <t>Author</t>
   </si>
@@ -94,9 +83,6 @@
   </si>
   <si>
     <t>Mahmoud Abdelmageed</t>
-  </si>
-  <si>
-    <t>Open</t>
   </si>
   <si>
     <t>LH-TC-NOTIGICATION-REVIEW-002</t>
@@ -184,6 +170,12 @@
   </si>
   <si>
     <t>Closed</t>
+  </si>
+  <si>
+    <t>v1.2</t>
+  </si>
+  <si>
+    <t>Verified Test cases after update</t>
   </si>
 </sst>
 </file>
@@ -707,9 +699,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -747,7 +739,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -853,7 +845,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -995,7 +987,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1005,26 +997,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="45.5546875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="36.6640625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="26.6640625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="21.109375" style="5" customWidth="1"/>
-    <col min="6" max="6" width="115.6640625" style="10" customWidth="1"/>
-    <col min="7" max="7" width="103.44140625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="28.33203125" style="5" customWidth="1"/>
-    <col min="9" max="9" width="19.5546875" style="5" customWidth="1"/>
-    <col min="10" max="10" width="37.44140625" style="5" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="5"/>
+    <col min="1" max="1" width="16.5703125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="45.5703125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="36.7109375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="115.7109375" style="10" customWidth="1"/>
+    <col min="7" max="7" width="103.42578125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="28.28515625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="19.5703125" style="5" customWidth="1"/>
+    <col min="10" max="10" width="37.42578125" style="5" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -1056,7 +1048,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="84" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" ht="84" x14ac:dyDescent="0.35">
       <c r="A2" s="11">
         <v>45768</v>
       </c>
@@ -1073,30 +1065,30 @@
         <v>2</v>
       </c>
       <c r="F2" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>28</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>29</v>
       </c>
       <c r="H2" s="12" t="s">
         <v>18</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="84" x14ac:dyDescent="0.4">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="84" x14ac:dyDescent="0.35">
       <c r="A3" s="11">
         <v>45768</v>
       </c>
       <c r="B3" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="12" t="s">
         <v>20</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>21</v>
       </c>
       <c r="D3" s="12" t="s">
         <v>15</v>
@@ -1105,30 +1097,30 @@
         <v>2</v>
       </c>
       <c r="F3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>22</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>23</v>
       </c>
       <c r="H3" s="12" t="s">
         <v>18</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="105" x14ac:dyDescent="0.4">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="105" x14ac:dyDescent="0.35">
       <c r="A4" s="11">
         <v>45768</v>
       </c>
       <c r="B4" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="12" t="s">
         <v>24</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>25</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>15</v>
@@ -1137,22 +1129,22 @@
         <v>2</v>
       </c>
       <c r="F4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>26</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>27</v>
       </c>
       <c r="H4" s="12" t="s">
         <v>18</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="8"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -1164,7 +1156,7 @@
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="8"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -1176,7 +1168,7 @@
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="8"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -1188,7 +1180,7 @@
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="8"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -1200,7 +1192,7 @@
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="8"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -1212,7 +1204,7 @@
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="8"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -1224,7 +1216,7 @@
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="8"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -1236,7 +1228,7 @@
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="8"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -1248,10 +1240,10 @@
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="9"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="9"/>
     </row>
   </sheetData>
@@ -1279,19 +1271,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.109375" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" customWidth="1"/>
-    <col min="3" max="3" width="36.5546875" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="36.5703125" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -1305,7 +1297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1316,56 +1308,65 @@
         <v>3</v>
       </c>
       <c r="D2" s="4">
-        <f t="shared" ref="D2:D9" si="0">DATE(2025,4,21)</f>
+        <f t="shared" ref="D2:D4" si="0">DATE(2025,4,21)</f>
         <v>45768</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D3" s="4">
         <f t="shared" si="0"/>
         <v>45768</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="4">
+        <f t="shared" si="0"/>
+        <v>45768</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>

</xml_diff>

<commit_message>
v2.1 reviewed and closed reviewer verification for notification testcases
LH_TC_NOTIFICATION_REVIEW
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_TC_NOTIFICATION_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_TC_NOTIFICATION_REVIEWS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gehad\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mego\Downloads\Group-3-Learning-hub-dev (1)\Group-3-Learning-hub-dev\LH_REVIEWS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4AF8873-362A-4939-A271-0A8D0DB8BF85}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D155D2C0-B793-4C25-A0A7-1E6C656DD53C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LH_TC_NOTIFICATION_REVIEWS" sheetId="2" r:id="rId1"/>
@@ -21,12 +21,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="44">
   <si>
     <t>Author</t>
   </si>
@@ -176,6 +187,37 @@
   </si>
   <si>
     <t>Verified Test cases after update</t>
+  </si>
+  <si>
+    <t>V2.0</t>
+  </si>
+  <si>
+    <t>Reviewed v2.0</t>
+  </si>
+  <si>
+    <t>V2.1</t>
+  </si>
+  <si>
+    <t>closed reviewer status</t>
+  </si>
+  <si>
+    <t>LH-TC-NOTIFICATION-005
+LH-TC-NOTIFICATION-003</t>
+  </si>
+  <si>
+    <t>LH-TC-NOTIGICATION-REVIEW-004</t>
+  </si>
+  <si>
+    <t>v2.0</t>
+  </si>
+  <si>
+    <t>The notifications are not a dropdown</t>
+  </si>
+  <si>
+    <t>Adjust testcase so that the notifications are a section not a dropdown</t>
+  </si>
+  <si>
+    <t>Hala Eldaly</t>
   </si>
 </sst>
 </file>
@@ -285,7 +327,7 @@
   </cellStyles>
   <dxfs count="18">
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -595,7 +637,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
@@ -699,9 +741,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -739,7 +781,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -845,7 +887,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -987,7 +1029,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -997,26 +1039,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="45.5703125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="36.7109375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="26.7109375" style="5" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="115.7109375" style="10" customWidth="1"/>
-    <col min="7" max="7" width="103.42578125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="28.28515625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="19.5703125" style="5" customWidth="1"/>
-    <col min="10" max="10" width="37.42578125" style="5" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="16.5546875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="45.5546875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="36.6640625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="26.6640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="21.109375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="115.6640625" style="10" customWidth="1"/>
+    <col min="7" max="7" width="103.44140625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="28.33203125" style="5" customWidth="1"/>
+    <col min="9" max="9" width="19.5546875" style="5" customWidth="1"/>
+    <col min="10" max="10" width="37.44140625" style="5" customWidth="1"/>
+    <col min="11" max="16384" width="9.109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -1048,7 +1090,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="84" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="84" x14ac:dyDescent="0.4">
       <c r="A2" s="11">
         <v>45768</v>
       </c>
@@ -1080,7 +1122,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="84" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="84" x14ac:dyDescent="0.4">
       <c r="A3" s="11">
         <v>45768</v>
       </c>
@@ -1112,7 +1154,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="105" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="105" x14ac:dyDescent="0.4">
       <c r="A4" s="11">
         <v>45768</v>
       </c>
@@ -1144,19 +1186,39 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" s="8"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="42" x14ac:dyDescent="0.4">
+      <c r="A5" s="8">
+        <v>45789</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A6" s="8"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -1168,7 +1230,7 @@
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A7" s="8"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -1180,7 +1242,7 @@
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A8" s="8"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -1192,7 +1254,7 @@
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A9" s="8"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -1204,7 +1266,7 @@
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A10" s="8"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -1216,7 +1278,7 @@
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A11" s="8"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -1228,7 +1290,7 @@
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A12" s="8"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -1240,10 +1302,10 @@
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A13" s="9"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A14" s="9"/>
     </row>
   </sheetData>
@@ -1271,19 +1333,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" customWidth="1"/>
-    <col min="3" max="3" width="36.5703125" customWidth="1"/>
+    <col min="1" max="1" width="25.109375" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" customWidth="1"/>
+    <col min="3" max="3" width="36.5546875" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -1297,7 +1359,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1312,7 +1374,7 @@
         <v>45768</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>29</v>
       </c>
@@ -1327,7 +1389,7 @@
         <v>45768</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>32</v>
       </c>
@@ -1342,31 +1404,47 @@
         <v>45768</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="4"/>
-    </row>
-    <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="4"/>
-    </row>
-    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="4">
+        <v>45789</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="4">
+        <v>45789</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>

</xml_diff>

<commit_message>
v2.0 reviewed Notification testcases
LH_TC_NOTIFICATION_REVIEW
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_TC_NOTIFICATION_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_TC_NOTIFICATION_REVIEWS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mego\Downloads\Group-3-Learning-hub-dev (1)\Group-3-Learning-hub-dev\LH_REVIEWS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D56F71F-86FD-4FBB-94EC-F2D0A29393A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED10E160-9E42-43D6-93AF-0BCF6445023D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LH_TC_NOTIFICATION_REVIEWS" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="43">
   <si>
     <t>Author</t>
   </si>
@@ -186,12 +186,6 @@
     <t>Reviewed v2.0</t>
   </si>
   <si>
-    <t>V2.1</t>
-  </si>
-  <si>
-    <t>closed reviewer status</t>
-  </si>
-  <si>
     <t>LH-TC-NOTIFICATION-005
 LH-TC-NOTIFICATION-003</t>
   </si>
@@ -218,6 +212,9 @@
   </si>
   <si>
     <t>LH-REVIEW-TC-NOTIFICATION-003</t>
+  </si>
+  <si>
+    <t>Open</t>
   </si>
 </sst>
 </file>
@@ -727,7 +724,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:D9" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:D8" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Version Number" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Author" dataDxfId="2"/>
@@ -1039,8 +1036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B5" sqref="B2:B5"/>
+    <sheetView topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -1095,7 +1092,7 @@
         <v>45768</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>16</v>
@@ -1127,7 +1124,7 @@
         <v>45768</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>18</v>
@@ -1159,7 +1156,7 @@
         <v>45768</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>21</v>
@@ -1191,31 +1188,31 @@
         <v>45789</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>17</v>
       </c>
       <c r="E5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="H5" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="G5" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="H5" s="12" t="s">
-        <v>39</v>
-      </c>
       <c r="I5" s="12" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.4">
@@ -1331,10 +1328,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1418,19 +1415,11 @@
         <v>45789</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" s="4">
-        <v>45789</v>
-      </c>
+    <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="4"/>
     </row>
     <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
@@ -1443,12 +1432,6 @@
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="4"/>
-    </row>
-    <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>